<commit_message>
update xlsxTransform to vTransform
</commit_message>
<xml_diff>
--- a/data/specialthanks-afd.xlsx
+++ b/data/specialthanks-afd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\lifeRestart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8FD2ED-7EB2-4664-9439-36FF7B849B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C87A3F-F6AA-41A0-BC51-B5E75F700C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="465">
   <si>
     <t>group</t>
   </si>
@@ -1998,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D430"/>
+  <dimension ref="A1:D429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2039,13 +2039,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2053,7 +2050,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2061,7 +2058,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2069,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2077,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2085,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2093,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2101,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2109,7 +2106,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2117,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2125,7 +2122,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2133,7 +2130,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2141,10 +2141,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>264</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2152,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2160,7 +2157,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2168,34 +2165,34 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -2203,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -2211,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -2219,7 +2216,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -2227,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -2235,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -2243,7 +2240,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -2251,26 +2248,26 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -2278,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2286,7 +2283,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2294,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2302,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2310,7 +2307,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2318,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2326,7 +2323,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2334,7 +2331,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2342,7 +2339,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2350,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2358,7 +2355,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2366,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2374,7 +2371,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2382,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2390,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2398,7 +2395,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2406,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2414,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2422,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2430,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2438,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2446,7 +2443,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -2454,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -2462,7 +2459,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -2470,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2478,7 +2475,7 @@
         <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2486,7 +2483,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2494,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -2502,7 +2499,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2510,7 +2507,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -2518,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -2526,7 +2523,7 @@
         <v>2</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -2534,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -2542,7 +2539,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -2550,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -2558,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -2566,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -2574,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -2582,7 +2579,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -2590,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2598,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -2606,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -2614,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -2622,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -2630,26 +2627,26 @@
         <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -2657,7 +2654,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -2665,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2673,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -2681,26 +2678,26 @@
         <v>2</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2708,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -2716,7 +2713,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -2724,7 +2721,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -2732,7 +2729,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -2740,7 +2737,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -2748,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2756,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -2764,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -2772,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -2780,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2788,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2796,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2804,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -2812,7 +2809,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -2820,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -2828,7 +2825,7 @@
         <v>2</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2836,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -2844,7 +2841,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -2852,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -2860,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -2868,7 +2865,7 @@
         <v>2</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -2876,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2884,7 +2881,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -2892,7 +2889,7 @@
         <v>2</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -2900,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -2908,15 +2905,18 @@
         <v>2</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -2924,21 +2924,18 @@
         <v>1</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -2946,7 +2943,7 @@
         <v>2</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -2954,7 +2951,7 @@
         <v>2</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -2962,7 +2959,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2970,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -2978,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2986,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -2994,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -3002,26 +2999,26 @@
         <v>2</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>322</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -3029,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -3037,7 +3034,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -3045,7 +3042,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -3053,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -3061,7 +3058,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -3069,7 +3066,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -3077,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -3085,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -3093,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -3101,7 +3098,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -3109,7 +3106,7 @@
         <v>2</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -3117,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -3125,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -3133,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -3141,23 +3138,23 @@
         <v>2</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>2</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>144</v>
+      <c r="B139" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>2</v>
       </c>
-      <c r="B140" s="3" t="s">
-        <v>286</v>
+      <c r="B140" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -3165,7 +3162,7 @@
         <v>2</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -3173,26 +3170,26 @@
         <v>2</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -3200,7 +3197,7 @@
         <v>2</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -3208,7 +3205,7 @@
         <v>2</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -3216,7 +3213,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -3224,7 +3221,7 @@
         <v>2</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -3232,7 +3229,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -3240,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -3248,7 +3245,7 @@
         <v>2</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -3256,7 +3253,7 @@
         <v>2</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -3264,7 +3261,7 @@
         <v>2</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -3272,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -3280,7 +3277,7 @@
         <v>2</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -3288,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -3296,7 +3293,7 @@
         <v>2</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -3304,7 +3301,7 @@
         <v>2</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -3312,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -3320,7 +3317,7 @@
         <v>2</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -3328,42 +3325,42 @@
         <v>2</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>2</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>167</v>
+      <c r="B162" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>2</v>
       </c>
-      <c r="B163" t="s">
-        <v>168</v>
+      <c r="B163" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -3371,7 +3368,7 @@
         <v>2</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -3379,15 +3376,18 @@
         <v>2</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -3395,10 +3395,10 @@
         <v>1</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -3406,21 +3406,18 @@
         <v>1</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -3428,7 +3425,7 @@
         <v>2</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -3436,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -3444,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -3452,7 +3449,7 @@
         <v>2</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -3460,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -3468,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -3476,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -3484,7 +3481,7 @@
         <v>2</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -3492,7 +3489,7 @@
         <v>2</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -3500,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -3508,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -3516,7 +3513,7 @@
         <v>2</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -3524,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -3532,7 +3529,7 @@
         <v>2</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3540,7 +3537,7 @@
         <v>2</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -3548,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -3556,7 +3553,7 @@
         <v>2</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -3564,7 +3561,7 @@
         <v>2</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -3572,26 +3569,26 @@
         <v>2</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>282</v>
+        <v>201</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -3599,7 +3596,7 @@
         <v>2</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -3607,7 +3604,7 @@
         <v>2</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -3615,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -3623,7 +3620,7 @@
         <v>2</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -3631,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -3639,7 +3636,7 @@
         <v>2</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -3647,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -3655,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -3663,7 +3660,7 @@
         <v>2</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -3671,7 +3668,7 @@
         <v>2</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -3679,7 +3676,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -3687,7 +3684,7 @@
         <v>2</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3695,7 +3692,7 @@
         <v>2</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -3703,7 +3700,7 @@
         <v>2</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -3711,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -3719,7 +3716,7 @@
         <v>2</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -3727,7 +3724,7 @@
         <v>2</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -3735,7 +3732,7 @@
         <v>2</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -3743,7 +3740,7 @@
         <v>2</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -3751,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -3759,62 +3756,62 @@
         <v>2</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>227</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="C217" s="2"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>2</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C218" s="2"/>
+        <v>229</v>
+      </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>2</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
@@ -3822,7 +3819,7 @@
         <v>2</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
@@ -3830,7 +3827,7 @@
         <v>2</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
@@ -3838,7 +3835,7 @@
         <v>2</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -3846,7 +3843,7 @@
         <v>2</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -3854,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
@@ -3862,7 +3859,7 @@
         <v>2</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
@@ -3870,26 +3867,26 @@
         <v>2</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
@@ -3897,7 +3894,7 @@
         <v>2</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -3905,7 +3902,7 @@
         <v>2</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
@@ -3913,7 +3910,7 @@
         <v>2</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
@@ -3921,7 +3918,7 @@
         <v>2</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
@@ -3929,7 +3926,7 @@
         <v>2</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
@@ -3937,7 +3934,7 @@
         <v>2</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
@@ -3945,7 +3942,7 @@
         <v>2</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -3953,15 +3950,15 @@
         <v>2</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>2</v>
       </c>
-      <c r="B237" s="1" t="s">
-        <v>248</v>
+      <c r="B237" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -3969,7 +3966,7 @@
         <v>2</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
@@ -3977,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
@@ -3985,7 +3982,7 @@
         <v>2</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
@@ -3993,26 +3990,26 @@
         <v>2</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C243" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
@@ -4020,7 +4017,7 @@
         <v>2</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
@@ -4028,7 +4025,7 @@
         <v>2</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -4036,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
@@ -4044,7 +4041,7 @@
         <v>2</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
@@ -4052,7 +4049,7 @@
         <v>2</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
@@ -4060,7 +4057,7 @@
         <v>2</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
@@ -4068,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
@@ -4076,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
@@ -4084,26 +4081,26 @@
         <v>2</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C254" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
@@ -4111,7 +4108,7 @@
         <v>2</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
@@ -4119,7 +4116,7 @@
         <v>2</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
@@ -4127,7 +4124,7 @@
         <v>2</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
@@ -4135,7 +4132,7 @@
         <v>2</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
@@ -4143,7 +4140,7 @@
         <v>2</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
@@ -4151,26 +4148,26 @@
         <v>2</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C262" s="3" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -4178,26 +4175,26 @@
         <v>2</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>278</v>
+        <v>280</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
@@ -4205,15 +4202,15 @@
         <v>2</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>2</v>
       </c>
-      <c r="B267" s="3" t="s">
-        <v>285</v>
+      <c r="B267" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
@@ -4221,15 +4218,15 @@
         <v>2</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>2</v>
       </c>
-      <c r="B269" s="1" t="s">
-        <v>288</v>
+      <c r="B269" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
@@ -4237,7 +4234,7 @@
         <v>2</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
@@ -4245,7 +4242,7 @@
         <v>2</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4253,23 +4250,23 @@
         <v>2</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>2</v>
       </c>
-      <c r="B273" s="3" t="s">
-        <v>292</v>
+      <c r="B273" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>2</v>
       </c>
-      <c r="B274" s="1" t="s">
-        <v>293</v>
+      <c r="B274" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
@@ -4277,7 +4274,7 @@
         <v>2</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4285,7 +4282,7 @@
         <v>2</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
@@ -4293,7 +4290,7 @@
         <v>2</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4301,23 +4298,23 @@
         <v>2</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>2</v>
       </c>
-      <c r="B279" s="3" t="s">
-        <v>298</v>
+      <c r="B279" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>2</v>
       </c>
-      <c r="B280" s="1" t="s">
-        <v>299</v>
+      <c r="B280" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
@@ -4325,7 +4322,7 @@
         <v>2</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
@@ -4333,7 +4330,7 @@
         <v>2</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
@@ -4341,7 +4338,7 @@
         <v>2</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
@@ -4349,7 +4346,7 @@
         <v>2</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
@@ -4357,26 +4354,26 @@
         <v>2</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C287" s="3" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
@@ -4384,7 +4381,7 @@
         <v>2</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
@@ -4392,7 +4389,7 @@
         <v>2</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
@@ -4400,7 +4397,7 @@
         <v>2</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
@@ -4408,7 +4405,7 @@
         <v>2</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
@@ -4416,7 +4413,7 @@
         <v>2</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
@@ -4424,7 +4421,7 @@
         <v>2</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
@@ -4432,7 +4429,7 @@
         <v>2</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
@@ -4440,7 +4437,7 @@
         <v>2</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
@@ -4448,7 +4445,7 @@
         <v>2</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
@@ -4456,7 +4453,7 @@
         <v>2</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
@@ -4464,7 +4461,7 @@
         <v>2</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
@@ -4472,7 +4469,7 @@
         <v>2</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
@@ -4480,7 +4477,7 @@
         <v>2</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
@@ -4488,26 +4485,26 @@
         <v>2</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C303" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
@@ -4515,7 +4512,7 @@
         <v>2</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
@@ -4523,7 +4520,7 @@
         <v>2</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
@@ -4531,7 +4528,7 @@
         <v>2</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
@@ -4539,7 +4536,7 @@
         <v>2</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
@@ -4547,7 +4544,7 @@
         <v>2</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
@@ -4555,7 +4552,7 @@
         <v>2</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
@@ -4563,7 +4560,7 @@
         <v>2</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
@@ -4571,7 +4568,7 @@
         <v>2</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -4579,7 +4576,7 @@
         <v>2</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -4587,7 +4584,7 @@
         <v>2</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
@@ -4595,7 +4592,7 @@
         <v>2</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
@@ -4603,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -4611,7 +4608,7 @@
         <v>2</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
@@ -4619,7 +4616,7 @@
         <v>2</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -4627,7 +4624,7 @@
         <v>2</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
@@ -4635,7 +4632,7 @@
         <v>2</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
@@ -4643,7 +4640,7 @@
         <v>2</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
@@ -4651,7 +4648,7 @@
         <v>2</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -4659,7 +4656,7 @@
         <v>2</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -4667,7 +4664,7 @@
         <v>2</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -4675,7 +4672,7 @@
         <v>2</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -4683,7 +4680,7 @@
         <v>2</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -4691,7 +4688,7 @@
         <v>2</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -4699,7 +4696,7 @@
         <v>2</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
@@ -4707,7 +4704,7 @@
         <v>2</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -4715,7 +4712,7 @@
         <v>2</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
@@ -4723,7 +4720,7 @@
         <v>2</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -4731,7 +4728,7 @@
         <v>2</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -4739,7 +4736,7 @@
         <v>2</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -4747,7 +4744,7 @@
         <v>2</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -4755,7 +4752,7 @@
         <v>2</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -4763,7 +4760,7 @@
         <v>2</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>357</v>
+        <v>385</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -4771,7 +4768,7 @@
         <v>2</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -4779,7 +4776,7 @@
         <v>2</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
@@ -4787,7 +4784,7 @@
         <v>2</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -4795,7 +4792,7 @@
         <v>2</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
@@ -4803,7 +4800,7 @@
         <v>2</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
@@ -4811,7 +4808,7 @@
         <v>2</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
@@ -4819,26 +4816,26 @@
         <v>2</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C344" s="3" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
@@ -4846,7 +4843,7 @@
         <v>2</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
@@ -4854,7 +4851,7 @@
         <v>2</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
@@ -4862,7 +4859,7 @@
         <v>2</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
@@ -4870,7 +4867,7 @@
         <v>2</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
@@ -4878,7 +4875,7 @@
         <v>2</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
@@ -4886,7 +4883,7 @@
         <v>2</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
@@ -4894,7 +4891,7 @@
         <v>2</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
@@ -4902,7 +4899,7 @@
         <v>2</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.3">
@@ -4910,7 +4907,7 @@
         <v>2</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.3">
@@ -4918,7 +4915,7 @@
         <v>2</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.3">
@@ -4926,7 +4923,7 @@
         <v>2</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.3">
@@ -4934,7 +4931,7 @@
         <v>2</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.3">
@@ -4942,7 +4939,7 @@
         <v>2</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.3">
@@ -4950,7 +4947,7 @@
         <v>2</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.3">
@@ -4958,7 +4955,7 @@
         <v>2</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.3">
@@ -4966,7 +4963,7 @@
         <v>2</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.3">
@@ -4974,7 +4971,7 @@
         <v>2</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.3">
@@ -4982,26 +4979,26 @@
         <v>2</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C364" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.3">
@@ -5009,7 +5006,7 @@
         <v>2</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.3">
@@ -5017,7 +5014,10 @@
         <v>2</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
+      </c>
+      <c r="D366" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.3">
@@ -5025,10 +5025,7 @@
         <v>2</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D367" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">
@@ -5036,7 +5033,7 @@
         <v>2</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
@@ -5044,7 +5041,7 @@
         <v>2</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
@@ -5052,7 +5049,7 @@
         <v>2</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
@@ -5060,7 +5057,7 @@
         <v>2</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
@@ -5068,7 +5065,7 @@
         <v>2</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -5076,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -5084,7 +5081,7 @@
         <v>2</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
@@ -5092,7 +5089,7 @@
         <v>2</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
@@ -5100,7 +5097,7 @@
         <v>2</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -5108,7 +5105,7 @@
         <v>2</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
@@ -5116,7 +5113,7 @@
         <v>2</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -5124,7 +5121,7 @@
         <v>2</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -5132,7 +5129,7 @@
         <v>2</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
@@ -5140,7 +5137,7 @@
         <v>2</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
@@ -5148,26 +5145,26 @@
         <v>2</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
+      </c>
+      <c r="C383" s="3" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C384" s="3" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
@@ -5175,7 +5172,7 @@
         <v>2</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.3">
@@ -5183,42 +5180,42 @@
         <v>2</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
+      </c>
+      <c r="C387" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="C388" s="3" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>2</v>
       </c>
-      <c r="B389" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="390" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B389" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" s="1">
         <v>2</v>
       </c>
-      <c r="B390" s="4" t="s">
-        <v>414</v>
+      <c r="B390" s="3" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
@@ -5226,29 +5223,29 @@
         <v>2</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A392" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>424</v>
+        <v>416</v>
+      </c>
+      <c r="C392" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D392" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="C393" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="D393" s="3" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
@@ -5256,7 +5253,7 @@
         <v>2</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
@@ -5264,7 +5261,7 @@
         <v>2</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
@@ -5272,7 +5269,7 @@
         <v>2</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -5280,7 +5277,7 @@
         <v>2</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -5288,29 +5285,29 @@
         <v>2</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="C399" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D399" s="3" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
-        <v>1</v>
-      </c>
-      <c r="B400" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="C400" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="D400" s="3" t="s">
-        <v>429</v>
+        <v>2</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
@@ -5318,7 +5315,7 @@
         <v>2</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
@@ -5326,7 +5323,7 @@
         <v>2</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
@@ -5334,7 +5331,7 @@
         <v>2</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
@@ -5342,7 +5339,7 @@
         <v>2</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
@@ -5350,7 +5347,7 @@
         <v>2</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
@@ -5358,7 +5355,7 @@
         <v>2</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
@@ -5366,7 +5363,7 @@
         <v>2</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
@@ -5374,7 +5371,7 @@
         <v>2</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
@@ -5382,7 +5379,7 @@
         <v>2</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
@@ -5390,7 +5387,7 @@
         <v>2</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
@@ -5398,26 +5395,26 @@
         <v>2</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
+      </c>
+      <c r="C412" s="3" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C413" s="3" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
@@ -5425,7 +5422,7 @@
         <v>2</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
@@ -5433,7 +5430,7 @@
         <v>2</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
@@ -5441,7 +5438,7 @@
         <v>2</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.3">
@@ -5449,7 +5446,7 @@
         <v>2</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
@@ -5457,7 +5454,7 @@
         <v>2</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
@@ -5465,26 +5462,26 @@
         <v>2</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
+      </c>
+      <c r="C420" s="3" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="C421" s="3" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
@@ -5492,26 +5489,26 @@
         <v>2</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
+      </c>
+      <c r="C423" s="3" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
-        <v>1</v>
-      </c>
-      <c r="B424" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C424" s="3" t="s">
-        <v>464</v>
+        <v>2</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
@@ -5519,7 +5516,7 @@
         <v>2</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
@@ -5527,42 +5524,34 @@
         <v>2</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
+      </c>
+      <c r="C427" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="C428" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
+      </c>
+      <c r="C428" s="3"/>
+      <c r="D428" s="3" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A429" s="1">
-        <v>2</v>
-      </c>
-      <c r="B429" s="3" t="s">
-        <v>461</v>
-      </c>
       <c r="C429" s="3"/>
-      <c r="D429" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C430" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>